<commit_message>
Changed Logic in saving test details.. and the format of test details xls.
</commit_message>
<xml_diff>
--- a/Education.WebApp/TestDetail/TestDetails.xlsx
+++ b/Education.WebApp/TestDetail/TestDetails.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Questions</t>
   </si>
@@ -30,32 +30,100 @@
     <t>Marks</t>
   </si>
   <si>
-    <t>OverLoad</t>
-  </si>
-  <si>
-    <t>Narendra Modi</t>
-  </si>
-  <si>
-    <t>Ram Nath Kovind</t>
-  </si>
-  <si>
-    <t>Object orieted</t>
-  </si>
-  <si>
-    <t>who is Prime Minister of India?</t>
+    <t>Higher per capita income of the people of the country</t>
+  </si>
+  <si>
+    <t>Higher shar of agricultur sector in the GDP of the country</t>
+  </si>
+  <si>
+    <t>Higher shar of industrial sector in the GDP of the country</t>
+  </si>
+  <si>
+    <t>Higher percentage of agriculture dependent population in the country</t>
+  </si>
+  <si>
+    <t>120 meters</t>
+  </si>
+  <si>
+    <t>100meters</t>
+  </si>
+  <si>
+    <t>300meters</t>
+  </si>
+  <si>
+    <t>400meters</t>
+  </si>
+  <si>
+    <t>45kmph</t>
+  </si>
+  <si>
+    <t>50kpmd</t>
+  </si>
+  <si>
+    <t>60kpmh</t>
+  </si>
+  <si>
+    <t>70kmpd</t>
+  </si>
+  <si>
+    <t>200m</t>
+  </si>
+  <si>
+    <t>100m</t>
+  </si>
+  <si>
+    <t>300m</t>
+  </si>
+  <si>
+    <t>500m</t>
+  </si>
+  <si>
+    <t>TEst1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5A5A5A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,14 +143,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,15 +457,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -408,24 +485,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -435,9 +509,6 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -449,9 +520,6 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -462,8 +530,223 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -471,9 +754,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D19" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit new code to branch
</commit_message>
<xml_diff>
--- a/Education.WebApp/TestDetail/TestDetails.xlsx
+++ b/Education.WebApp/TestDetail/TestDetails.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Questions</t>
   </si>
@@ -30,100 +30,32 @@
     <t>Marks</t>
   </si>
   <si>
-    <t>Higher per capita income of the people of the country</t>
-  </si>
-  <si>
-    <t>Higher shar of agricultur sector in the GDP of the country</t>
-  </si>
-  <si>
-    <t>Higher shar of industrial sector in the GDP of the country</t>
-  </si>
-  <si>
-    <t>Higher percentage of agriculture dependent population in the country</t>
-  </si>
-  <si>
-    <t>120 meters</t>
-  </si>
-  <si>
-    <t>100meters</t>
-  </si>
-  <si>
-    <t>300meters</t>
-  </si>
-  <si>
-    <t>400meters</t>
-  </si>
-  <si>
-    <t>45kmph</t>
-  </si>
-  <si>
-    <t>50kpmd</t>
-  </si>
-  <si>
-    <t>60kpmh</t>
-  </si>
-  <si>
-    <t>70kmpd</t>
-  </si>
-  <si>
-    <t>200m</t>
-  </si>
-  <si>
-    <t>100m</t>
-  </si>
-  <si>
-    <t>300m</t>
-  </si>
-  <si>
-    <t>500m</t>
-  </si>
-  <si>
-    <t>TEst1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
+    <t>OverLoad</t>
+  </si>
+  <si>
+    <t>Narendra Modi</t>
+  </si>
+  <si>
+    <t>Ram Nath Kovind</t>
+  </si>
+  <si>
+    <t>Object orieted</t>
+  </si>
+  <si>
+    <t>who is Prime Minister of India?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Georgia"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF5A5A5A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,22 +75,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,16 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -485,10 +408,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -498,8 +421,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -509,6 +435,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -520,6 +449,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -529,224 +461,9 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -754,17 +471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D19" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="91.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>